<commit_message>
update to the lock state excel
</commit_message>
<xml_diff>
--- a/halkomatic_lock_states_beiarntek.xlsx
+++ b/halkomatic_lock_states_beiarntek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\koulu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBF87B1E-628F-4AC0-ACBC-87A7ECEAAD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BF56645-0513-4108-BF2E-818383E98016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="2295" windowWidth="24825" windowHeight="15345" xr2:uid="{F03F0F33-F6BC-4382-A6CD-1C74174D72E9}"/>
+    <workbookView xWindow="3870" yWindow="4860" windowWidth="33765" windowHeight="15345" xr2:uid="{F03F0F33-F6BC-4382-A6CD-1C74174D72E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2057" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="37">
   <si>
     <t>O</t>
   </si>
@@ -60,6 +60,93 @@
   </si>
   <si>
     <t>BIN</t>
+  </si>
+  <si>
+    <t>02 00 00 65 07 00 00 00 00 C0 03 31</t>
+  </si>
+  <si>
+    <t>.03</t>
+  </si>
+  <si>
+    <t>.02</t>
+  </si>
+  <si>
+    <t>.00</t>
+  </si>
+  <si>
+    <t>.65</t>
+  </si>
+  <si>
+    <t>example return data of lock status:</t>
+  </si>
+  <si>
+    <t>.07</t>
+  </si>
+  <si>
+    <t>.c0</t>
+  </si>
+  <si>
+    <t>sum check</t>
+  </si>
+  <si>
+    <t>CU adress</t>
+  </si>
+  <si>
+    <t>"nonsense"</t>
+  </si>
+  <si>
+    <t>command</t>
+  </si>
+  <si>
+    <t>locks 1-8</t>
+  </si>
+  <si>
+    <t>locks 9-16</t>
+  </si>
+  <si>
+    <t>locks 17-24</t>
+  </si>
+  <si>
+    <t>locks 25-32</t>
+  </si>
+  <si>
+    <t>locks 33-40</t>
+  </si>
+  <si>
+    <t>locks 41-48</t>
+  </si>
+  <si>
+    <t>end (constant)</t>
+  </si>
+  <si>
+    <t>start (constant)</t>
+  </si>
+  <si>
+    <t>in the example the closed locks are:</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 47 and 48</t>
+  </si>
+  <si>
+    <t>1, 2, 3</t>
+  </si>
+  <si>
+    <t>47, 48</t>
+  </si>
+  <si>
+    <t>all other locks are open</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>dec</t>
+  </si>
+  <si>
+    <t>this is smaller because of the sum being past 255</t>
+  </si>
+  <si>
+    <t>sum seems to reset to "0" when going past "255" or "FF"</t>
   </si>
 </sst>
 </file>
@@ -310,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -333,6 +420,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -672,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFF1AD1-6196-4A98-A534-70B88BAE52A4}">
-  <dimension ref="A1:K257"/>
+  <dimension ref="A1:Z257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,10 +778,21 @@
     <col min="9" max="9" width="18.85546875" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
     <col min="11" max="11" width="15.5703125" customWidth="1"/>
-    <col min="14" max="14" width="69.28515625" customWidth="1"/>
+    <col min="14" max="14" width="72" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" customWidth="1"/>
+    <col min="20" max="20" width="10.42578125" customWidth="1"/>
+    <col min="21" max="21" width="11.140625" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" customWidth="1"/>
+    <col min="23" max="23" width="11" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" customWidth="1"/>
+    <col min="25" max="25" width="13.5703125" customWidth="1"/>
+    <col min="26" max="26" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -696,7 +802,7 @@
       <c r="C1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="9"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
@@ -706,7 +812,7 @@
       <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="11" t="s">
         <v>3</v>
       </c>
@@ -717,7 +823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -752,7 +858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
@@ -788,8 +894,47 @@
         <f>DEC2BIN(I3)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N3" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="23">
+        <v>1</v>
+      </c>
+      <c r="P3" s="23">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>3</v>
+      </c>
+      <c r="R3" s="23">
+        <v>4</v>
+      </c>
+      <c r="S3" s="23">
+        <v>5</v>
+      </c>
+      <c r="T3" s="23">
+        <v>6</v>
+      </c>
+      <c r="U3" s="23">
+        <v>7</v>
+      </c>
+      <c r="V3" s="23">
+        <v>8</v>
+      </c>
+      <c r="W3" s="23">
+        <v>9</v>
+      </c>
+      <c r="X3" s="23">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="23">
+        <v>11</v>
+      </c>
+      <c r="Z3" s="23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -825,8 +970,47 @@
         <f t="shared" ref="K4:K67" si="1">DEC2BIN(I4)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N4" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="T4" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>0</v>
       </c>
@@ -862,8 +1046,47 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N5" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -899,8 +1122,47 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N6" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="12">
+        <v>2</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>0</v>
+      </c>
+      <c r="R6" s="24">
+        <v>101</v>
+      </c>
+      <c r="S6" s="12">
+        <v>7</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="12">
+        <v>0</v>
+      </c>
+      <c r="V6" s="1">
+        <v>0</v>
+      </c>
+      <c r="W6" s="12">
+        <v>0</v>
+      </c>
+      <c r="X6" s="1">
+        <v>192</v>
+      </c>
+      <c r="Y6" s="12">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
@@ -936,8 +1198,20 @@
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N7" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="S7" t="s">
+        <v>30</v>
+      </c>
+      <c r="X7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -973,8 +1247,11 @@
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +1288,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1047,8 +1324,11 @@
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N10" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>0</v>
       </c>
@@ -1085,7 +1365,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1121,8 +1401,11 @@
         <f t="shared" si="1"/>
         <v>1010</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N12" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>0</v>
       </c>
@@ -1159,7 +1442,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1196,7 +1479,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>0</v>
       </c>
@@ -1233,7 +1516,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>